<commit_message>
Funções cont.se e somase
</commit_message>
<xml_diff>
--- a/02-Meteora_Ecommerce _Funcoes.xlsx
+++ b/02-Meteora_Ecommerce _Funcoes.xlsx
@@ -8,28 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\Meu Drive (mz.tears.of.time@gmail.com)\Dev\Cursos\Curso-003\001 - Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77ABF397-43DE-4632-B22B-CBAF2CBEC2EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D292C8-F2B8-4DF4-97BA-22B0E1A586F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33330" yWindow="-120" windowWidth="20640" windowHeight="11040" activeTab="3" xr2:uid="{F6D97A53-F63B-4272-A181-44B26E0B790F}"/>
+    <workbookView xWindow="34260" yWindow="-120" windowWidth="20640" windowHeight="11040" firstSheet="1" activeTab="3" xr2:uid="{F6D97A53-F63B-4272-A181-44B26E0B790F}"/>
   </bookViews>
   <sheets>
     <sheet name="Meu Gráfico" sheetId="6" r:id="rId1"/>
     <sheet name="Planilha3" sheetId="5" r:id="rId2"/>
     <sheet name="Produtos" sheetId="1" r:id="rId3"/>
-    <sheet name="Filtro_Avançado" sheetId="8" r:id="rId4"/>
-    <sheet name="Produtos (Com Tabela)" sheetId="2" r:id="rId5"/>
-    <sheet name="Obs" sheetId="7" r:id="rId6"/>
+    <sheet name="Planilha1" sheetId="9" r:id="rId4"/>
+    <sheet name="Filtro_Avançado" sheetId="8" r:id="rId5"/>
+    <sheet name="Produtos (Com Tabela)" sheetId="2" r:id="rId6"/>
+    <sheet name="Planilha2" sheetId="10" r:id="rId7"/>
+    <sheet name="Obs" sheetId="7" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Produtos!$A$3:$G$42</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="3">Filtro_Avançado!$B$6:$H$6</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="4">Filtro_Avançado!$B$6:$H$6</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Produtos!$A$1:$I$44</definedName>
-    <definedName name="_xlnm.Criteria" localSheetId="3">Filtro_Avançado!$B$2:$C$3</definedName>
+    <definedName name="_xlnm.Criteria" localSheetId="4">Filtro_Avançado!$B$2:$C$3</definedName>
+    <definedName name="Int_Nome_Produto">Produtos!$A$4:$A$42</definedName>
+    <definedName name="Int_Nome_Produtos">Produtos!$A$4:$A$42</definedName>
+    <definedName name="int_Qtd">Produtos!$F$4:$F$42</definedName>
     <definedName name="Produtos">Produtos!$A$3:$A$42</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="48">
   <si>
     <t>Produtos</t>
   </si>
@@ -170,6 +175,21 @@
   <si>
     <t>&lt;12</t>
   </si>
+  <si>
+    <t>Meus Números</t>
+  </si>
+  <si>
+    <t>dashboard'</t>
+  </si>
+  <si>
+    <t>Contagem de Produtos</t>
+  </si>
+  <si>
+    <t>Soma de Qtde em Estoque</t>
+  </si>
+  <si>
+    <t>Tênis*</t>
+  </si>
 </sst>
 </file>
 
@@ -178,7 +198,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,8 +281,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -293,6 +345,12 @@
         <bgColor theme="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="23">
     <border>
@@ -619,7 +677,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -690,6 +748,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -702,14 +769,22 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2087,7 +2162,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{8D58BA28-6F2B-4BE7-9135-3BC55F666805}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="109" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="101" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -2098,7 +2173,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9656078" cy="6020849"/>
+    <xdr:ext cx="9640957" cy="6013174"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -3035,7 +3110,7 @@
   <dimension ref="A3:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3206,8 +3281,9 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="91" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3:F4"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="C45" sqref="C45"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3223,15 +3299,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
     </row>
     <row r="2" spans="1:9" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3"/>
@@ -3282,14 +3358,14 @@
         <v>65.900000000000006</v>
       </c>
       <c r="E4" s="19">
-        <f>D4-(D4*$I$4)</f>
+        <f t="shared" ref="E4:E42" si="0">D4-(D4*$I$4)</f>
         <v>59.31</v>
       </c>
       <c r="F4" s="20">
         <v>12</v>
       </c>
       <c r="G4" s="19">
-        <f>E4*F4</f>
+        <f t="shared" ref="G4:G42" si="1">E4*F4</f>
         <v>711.72</v>
       </c>
       <c r="I4" s="30">
@@ -3310,14 +3386,14 @@
         <v>69.900000000000006</v>
       </c>
       <c r="E5" s="17">
-        <f>D5-(D5*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>62.910000000000004</v>
       </c>
       <c r="F5" s="21">
         <v>15</v>
       </c>
       <c r="G5" s="17">
-        <f>E5*F5</f>
+        <f t="shared" si="1"/>
         <v>943.65000000000009</v>
       </c>
     </row>
@@ -3335,14 +3411,14 @@
         <v>70.900000000000006</v>
       </c>
       <c r="E6" s="17">
-        <f>D6-(D6*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>63.81</v>
       </c>
       <c r="F6" s="21">
         <v>13</v>
       </c>
       <c r="G6" s="17">
-        <f>E6*F6</f>
+        <f t="shared" si="1"/>
         <v>829.53</v>
       </c>
     </row>
@@ -3360,14 +3436,14 @@
         <v>145</v>
       </c>
       <c r="E7" s="19">
-        <f>D7-(D7*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>130.5</v>
       </c>
       <c r="F7" s="20">
         <v>2</v>
       </c>
       <c r="G7" s="19">
-        <f>E7*F7</f>
+        <f t="shared" si="1"/>
         <v>261</v>
       </c>
     </row>
@@ -3385,14 +3461,14 @@
         <v>259.89999999999998</v>
       </c>
       <c r="E8" s="17">
-        <f>D8-(D8*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>233.90999999999997</v>
       </c>
       <c r="F8" s="21">
         <v>1</v>
       </c>
       <c r="G8" s="17">
-        <f>E8*F8</f>
+        <f t="shared" si="1"/>
         <v>233.90999999999997</v>
       </c>
     </row>
@@ -3410,14 +3486,14 @@
         <v>39.9</v>
       </c>
       <c r="E9" s="17">
-        <f>D9-(D9*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>35.909999999999997</v>
       </c>
       <c r="F9" s="21">
         <v>11</v>
       </c>
       <c r="G9" s="17">
-        <f>E9*F9</f>
+        <f t="shared" si="1"/>
         <v>395.01</v>
       </c>
     </row>
@@ -3435,14 +3511,14 @@
         <v>85.9</v>
       </c>
       <c r="E10" s="17">
-        <f>D10-(D10*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>77.31</v>
       </c>
       <c r="F10" s="21">
         <v>8</v>
       </c>
       <c r="G10" s="17">
-        <f>E10*F10</f>
+        <f t="shared" si="1"/>
         <v>618.48</v>
       </c>
     </row>
@@ -3460,14 +3536,14 @@
         <v>89.9</v>
       </c>
       <c r="E11" s="17">
-        <f>D11-(D11*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>80.910000000000011</v>
       </c>
       <c r="F11" s="21">
         <v>5</v>
       </c>
       <c r="G11" s="17">
-        <f>E11*F11</f>
+        <f t="shared" si="1"/>
         <v>404.55000000000007</v>
       </c>
     </row>
@@ -3485,14 +3561,14 @@
         <v>92.9</v>
       </c>
       <c r="E12" s="17">
-        <f>D12-(D12*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>83.61</v>
       </c>
       <c r="F12" s="21">
         <v>6</v>
       </c>
       <c r="G12" s="17">
-        <f>E12*F12</f>
+        <f t="shared" si="1"/>
         <v>501.65999999999997</v>
       </c>
     </row>
@@ -3510,14 +3586,14 @@
         <v>44.9</v>
       </c>
       <c r="E13" s="17">
-        <f>D13-(D13*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>40.409999999999997</v>
       </c>
       <c r="F13" s="21">
         <v>5</v>
       </c>
       <c r="G13" s="17">
-        <f>E13*F13</f>
+        <f t="shared" si="1"/>
         <v>202.04999999999998</v>
       </c>
     </row>
@@ -3535,14 +3611,14 @@
         <v>46.9</v>
       </c>
       <c r="E14" s="17">
-        <f>D14-(D14*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>42.21</v>
       </c>
       <c r="F14" s="21">
         <v>3</v>
       </c>
       <c r="G14" s="17">
-        <f>E14*F14</f>
+        <f t="shared" si="1"/>
         <v>126.63</v>
       </c>
     </row>
@@ -3560,14 +3636,14 @@
         <v>48.9</v>
       </c>
       <c r="E15" s="17">
-        <f>D15-(D15*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>44.01</v>
       </c>
       <c r="F15" s="21">
         <v>2</v>
       </c>
       <c r="G15" s="17">
-        <f>E15*F15</f>
+        <f t="shared" si="1"/>
         <v>88.02</v>
       </c>
     </row>
@@ -3585,14 +3661,14 @@
         <v>39.9</v>
       </c>
       <c r="E16" s="17">
-        <f>D16-(D16*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>35.909999999999997</v>
       </c>
       <c r="F16" s="21">
         <v>12</v>
       </c>
       <c r="G16" s="17">
-        <f>E16*F16</f>
+        <f t="shared" si="1"/>
         <v>430.91999999999996</v>
       </c>
     </row>
@@ -3610,14 +3686,14 @@
         <v>39.9</v>
       </c>
       <c r="E17" s="17">
-        <f>D17-(D17*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>35.909999999999997</v>
       </c>
       <c r="F17" s="21">
         <v>10</v>
       </c>
       <c r="G17" s="17">
-        <f>E17*F17</f>
+        <f t="shared" si="1"/>
         <v>359.09999999999997</v>
       </c>
     </row>
@@ -3635,14 +3711,14 @@
         <v>42.5</v>
       </c>
       <c r="E18" s="17">
-        <f>D18-(D18*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>38.25</v>
       </c>
       <c r="F18" s="21">
         <v>6</v>
       </c>
       <c r="G18" s="17">
-        <f>E18*F18</f>
+        <f t="shared" si="1"/>
         <v>229.5</v>
       </c>
     </row>
@@ -3660,14 +3736,14 @@
         <v>25.9</v>
       </c>
       <c r="E19" s="17">
-        <f>D19-(D19*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>23.31</v>
       </c>
       <c r="F19" s="21">
         <v>12</v>
       </c>
       <c r="G19" s="17">
-        <f>E19*F19</f>
+        <f t="shared" si="1"/>
         <v>279.71999999999997</v>
       </c>
     </row>
@@ -3685,14 +3761,14 @@
         <v>29.9</v>
       </c>
       <c r="E20" s="17">
-        <f>D20-(D20*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>26.909999999999997</v>
       </c>
       <c r="F20" s="21">
         <v>10</v>
       </c>
       <c r="G20" s="17">
-        <f>E20*F20</f>
+        <f t="shared" si="1"/>
         <v>269.09999999999997</v>
       </c>
     </row>
@@ -3710,14 +3786,14 @@
         <v>32.9</v>
       </c>
       <c r="E21" s="17">
-        <f>D21-(D21*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>29.61</v>
       </c>
       <c r="F21" s="21">
         <v>6</v>
       </c>
       <c r="G21" s="17">
-        <f>E21*F21</f>
+        <f t="shared" si="1"/>
         <v>177.66</v>
       </c>
     </row>
@@ -3735,14 +3811,14 @@
         <v>49.9</v>
       </c>
       <c r="E22" s="17">
-        <f>D22-(D22*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>44.91</v>
       </c>
       <c r="F22" s="21">
         <v>21</v>
       </c>
       <c r="G22" s="17">
-        <f>E22*F22</f>
+        <f t="shared" si="1"/>
         <v>943.1099999999999</v>
       </c>
     </row>
@@ -3760,14 +3836,14 @@
         <v>300</v>
       </c>
       <c r="E23" s="17">
-        <f>D23-(D23*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>270</v>
       </c>
       <c r="F23" s="21">
         <v>1</v>
       </c>
       <c r="G23" s="17">
-        <f>E23*F23</f>
+        <f t="shared" si="1"/>
         <v>270</v>
       </c>
     </row>
@@ -3785,14 +3861,14 @@
         <v>302.89999999999998</v>
       </c>
       <c r="E24" s="17">
-        <f>D24-(D24*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>272.60999999999996</v>
       </c>
       <c r="F24" s="21">
         <v>2</v>
       </c>
       <c r="G24" s="17">
-        <f>E24*F24</f>
+        <f t="shared" si="1"/>
         <v>545.21999999999991</v>
       </c>
     </row>
@@ -3810,14 +3886,14 @@
         <v>299.89999999999998</v>
       </c>
       <c r="E25" s="17">
-        <f>D25-(D25*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>269.90999999999997</v>
       </c>
       <c r="F25" s="21">
         <v>1</v>
       </c>
       <c r="G25" s="17">
-        <f>E25*F25</f>
+        <f t="shared" si="1"/>
         <v>269.90999999999997</v>
       </c>
     </row>
@@ -3835,14 +3911,14 @@
         <v>249.9</v>
       </c>
       <c r="E26" s="17">
-        <f>D26-(D26*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>224.91</v>
       </c>
       <c r="F26" s="21">
         <v>1</v>
       </c>
       <c r="G26" s="17">
-        <f>E26*F26</f>
+        <f t="shared" si="1"/>
         <v>224.91</v>
       </c>
     </row>
@@ -3860,14 +3936,14 @@
         <v>259.89999999999998</v>
       </c>
       <c r="E27" s="17">
-        <f>D27-(D27*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>233.90999999999997</v>
       </c>
       <c r="F27" s="21">
         <v>2</v>
       </c>
       <c r="G27" s="17">
-        <f>E27*F27</f>
+        <f t="shared" si="1"/>
         <v>467.81999999999994</v>
       </c>
     </row>
@@ -3885,14 +3961,14 @@
         <v>299.89999999999998</v>
       </c>
       <c r="E28" s="17">
-        <f>D28-(D28*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>269.90999999999997</v>
       </c>
       <c r="F28" s="21">
         <v>1</v>
       </c>
       <c r="G28" s="17">
-        <f>E28*F28</f>
+        <f t="shared" si="1"/>
         <v>269.90999999999997</v>
       </c>
     </row>
@@ -3910,14 +3986,14 @@
         <v>349.9</v>
       </c>
       <c r="E29" s="17">
-        <f>D29-(D29*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>314.90999999999997</v>
       </c>
       <c r="F29" s="21">
         <v>2</v>
       </c>
       <c r="G29" s="17">
-        <f>E29*F29</f>
+        <f t="shared" si="1"/>
         <v>629.81999999999994</v>
       </c>
     </row>
@@ -3935,14 +4011,14 @@
         <v>399.9</v>
       </c>
       <c r="E30" s="17">
-        <f>D30-(D30*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>359.90999999999997</v>
       </c>
       <c r="F30" s="21">
         <v>3</v>
       </c>
       <c r="G30" s="17">
-        <f>E30*F30</f>
+        <f t="shared" si="1"/>
         <v>1079.73</v>
       </c>
     </row>
@@ -3960,14 +4036,14 @@
         <v>249.9</v>
       </c>
       <c r="E31" s="17">
-        <f>D31-(D31*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>224.91</v>
       </c>
       <c r="F31" s="21">
         <v>5</v>
       </c>
       <c r="G31" s="17">
-        <f>E31*F31</f>
+        <f t="shared" si="1"/>
         <v>1124.55</v>
       </c>
     </row>
@@ -3985,14 +4061,14 @@
         <v>255</v>
       </c>
       <c r="E32" s="17">
-        <f>D32-(D32*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>229.5</v>
       </c>
       <c r="F32" s="21">
         <v>3</v>
       </c>
       <c r="G32" s="17">
-        <f>E32*F32</f>
+        <f t="shared" si="1"/>
         <v>688.5</v>
       </c>
     </row>
@@ -4010,14 +4086,14 @@
         <v>259.89999999999998</v>
       </c>
       <c r="E33" s="17">
-        <f>D33-(D33*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>233.90999999999997</v>
       </c>
       <c r="F33" s="21">
         <v>1</v>
       </c>
       <c r="G33" s="17">
-        <f>E33*F33</f>
+        <f t="shared" si="1"/>
         <v>233.90999999999997</v>
       </c>
     </row>
@@ -4035,14 +4111,14 @@
         <v>199.9</v>
       </c>
       <c r="E34" s="17">
-        <f>D34-(D34*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>179.91</v>
       </c>
       <c r="F34" s="21">
         <v>0</v>
       </c>
       <c r="G34" s="17">
-        <f>E34*F34</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4060,14 +4136,14 @@
         <v>249.9</v>
       </c>
       <c r="E35" s="17">
-        <f>D35-(D35*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>224.91</v>
       </c>
       <c r="F35" s="21">
         <v>1</v>
       </c>
       <c r="G35" s="17">
-        <f>E35*F35</f>
+        <f t="shared" si="1"/>
         <v>224.91</v>
       </c>
     </row>
@@ -4085,14 +4161,14 @@
         <v>259.89999999999998</v>
       </c>
       <c r="E36" s="17">
-        <f>D36-(D36*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>233.90999999999997</v>
       </c>
       <c r="F36" s="21">
         <v>0</v>
       </c>
       <c r="G36" s="17">
-        <f>E36*F36</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4110,14 +4186,14 @@
         <v>89.9</v>
       </c>
       <c r="E37" s="17">
-        <f>D37-(D37*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>80.910000000000011</v>
       </c>
       <c r="F37" s="21">
         <v>3</v>
       </c>
       <c r="G37" s="17">
-        <f>E37*F37</f>
+        <f t="shared" si="1"/>
         <v>242.73000000000002</v>
       </c>
     </row>
@@ -4135,14 +4211,14 @@
         <v>91.4</v>
       </c>
       <c r="E38" s="17">
-        <f>D38-(D38*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>82.26</v>
       </c>
       <c r="F38" s="21">
         <v>2</v>
       </c>
       <c r="G38" s="17">
-        <f>E38*F38</f>
+        <f t="shared" si="1"/>
         <v>164.52</v>
       </c>
     </row>
@@ -4160,14 +4236,14 @@
         <v>93.5</v>
       </c>
       <c r="E39" s="17">
-        <f>D39-(D39*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>84.15</v>
       </c>
       <c r="F39" s="21">
         <v>2</v>
       </c>
       <c r="G39" s="17">
-        <f>E39*F39</f>
+        <f t="shared" si="1"/>
         <v>168.3</v>
       </c>
     </row>
@@ -4185,14 +4261,14 @@
         <v>140</v>
       </c>
       <c r="E40" s="17">
-        <f>D40-(D40*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>126</v>
       </c>
       <c r="F40" s="21">
         <v>2</v>
       </c>
       <c r="G40" s="17">
-        <f>E40*F40</f>
+        <f t="shared" si="1"/>
         <v>252</v>
       </c>
     </row>
@@ -4210,14 +4286,14 @@
         <v>142.9</v>
       </c>
       <c r="E41" s="17">
-        <f>D41-(D41*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>128.61000000000001</v>
       </c>
       <c r="F41" s="21">
         <v>2</v>
       </c>
       <c r="G41" s="17">
-        <f>E41*F41</f>
+        <f t="shared" si="1"/>
         <v>257.22000000000003</v>
       </c>
     </row>
@@ -4235,14 +4311,14 @@
         <v>146</v>
       </c>
       <c r="E42" s="18">
-        <f>D42-(D42*$I$4)</f>
+        <f t="shared" si="0"/>
         <v>131.4</v>
       </c>
       <c r="F42" s="22">
         <v>2</v>
       </c>
       <c r="G42" s="18">
-        <f>E42*F42</f>
+        <f t="shared" si="1"/>
         <v>262.8</v>
       </c>
     </row>
@@ -4256,11 +4332,11 @@
       <c r="G43" s="3"/>
     </row>
     <row r="44" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="34" t="s">
+      <c r="A44" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="B44" s="35"/>
-      <c r="C44" s="36"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="39"/>
       <c r="D44" s="24">
         <f>SUM(D4:D42)</f>
         <v>5962.2999999999984</v>
@@ -4298,11 +4374,80 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D385B69-1D6D-4736-AA8C-E002AF1AD43B}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D2" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="46"/>
+    </row>
+    <row r="3" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="44">
+        <f>COUNTIF(Produtos!F4:F42,"&gt;0")</f>
+        <v>37</v>
+      </c>
+      <c r="C4" s="44">
+        <f>Produtos!F44</f>
+        <v>196</v>
+      </c>
+      <c r="D4" s="44">
+        <f>COUNTIF(Int_Nome_Produto,D2)</f>
+        <v>6</v>
+      </c>
+      <c r="E4" s="44">
+        <f>SUMIF(Int_Nome_Produto,D2,int_Qtd)</f>
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7326DF80-0DFA-4F65-BD4E-022C0B3B8C1C}">
   <dimension ref="B1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4317,15 +4462,15 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="35" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="36" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="22" t="s">
@@ -4545,12 +4690,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1525D4F-4FEE-4357-9658-5E1916B70D88}">
   <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4567,15 +4712,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
     </row>
     <row r="2" spans="1:9" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3"/>
@@ -5623,7 +5768,49 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0E530DD-BD21-46D7-8036-4A7C49A06075}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:3" ht="52.5" x14ac:dyDescent="0.25">
+      <c r="B3" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="44">
+        <f>COUNTIF(Tabela5[Qtd],"&gt;0")</f>
+        <v>37</v>
+      </c>
+      <c r="C4" s="44">
+        <f>Tabela5[[#Totals],[Qtd]]</f>
+        <v>196</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D76905C-547A-4F6E-A046-A2B2ECB578CD}">
   <dimension ref="A2:G4"/>
   <sheetViews>

</xml_diff>